<commit_message>
Finished updating data. Added future improvements section
</commit_message>
<xml_diff>
--- a/Datasheets/C_Gearboxes.xlsx
+++ b/Datasheets/C_Gearboxes.xlsx
@@ -415,7 +415,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.09765625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="2" style="1" width="12.11"/>
@@ -1908,7 +1908,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.09765625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="2" style="1" width="12.11"/>
@@ -4885,7 +4885,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.09765625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="2" style="1" width="12.11"/>
@@ -7809,7 +7809,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.09765625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="2" style="1" width="12.11"/>
@@ -10097,7 +10097,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.09765625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="2" style="1" width="12.11"/>
@@ -12385,7 +12385,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.09765625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="2" style="1" width="12.11"/>
@@ -15150,7 +15150,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.09765625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="2" style="1" width="12.11"/>
@@ -18233,7 +18233,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.09765625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="2" style="1" width="12.11"/>
@@ -21581,7 +21581,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.09765625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="2" style="1" width="12.11"/>
@@ -24611,7 +24611,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.09765625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="2" style="1" width="12.11"/>
@@ -27535,7 +27535,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.09765625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="2" style="1" width="12.11"/>

</xml_diff>